<commit_message>
Update Readme & Process_Data
</commit_message>
<xml_diff>
--- a/Dataset_inf.xlsx
+++ b/Dataset_inf.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="396">
   <si>
     <t>Note</t>
   </si>
@@ -1403,6 +1403,9 @@
   </si>
   <si>
     <t>Wang_2016_EPHPP</t>
+  </si>
+  <si>
+    <t>Pa2E1</t>
   </si>
 </sst>
 </file>
@@ -2466,10 +2469,10 @@
   <sheetPr/>
   <dimension ref="A1:KJ68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" topLeftCell="A37" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="AI1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -21264,8 +21267,12 @@
     </row>
     <row r="54" ht="15.5" spans="1:296">
       <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
+      <c r="B54" s="2">
+        <v>53</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>395</v>
+      </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
       <c r="F54" s="2"/>

</xml_diff>

<commit_message>
Update Clean_Data and Dataset_inf
</commit_message>
<xml_diff>
--- a/Dataset_inf.xlsx
+++ b/Dataset_inf.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="24750" windowHeight="10480"/>
+    <workbookView windowWidth="27950" windowHeight="12280"/>
   </bookViews>
   <sheets>
     <sheet name="Label" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Label!$A$1:$AK$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Label!$A$1:$AK$57</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="904" uniqueCount="409">
   <si>
     <t>Note</t>
   </si>
@@ -50,7 +50,7 @@
     <t>Questionnaire Data</t>
   </si>
   <si>
-    <t>EEG Data</t>
+    <t>EEG/fMRI Data</t>
   </si>
   <si>
     <t>Corresponding author</t>
@@ -1393,7 +1393,7 @@
     <t>https://doi.org/10.3758/s13415-024-01157-0.</t>
   </si>
   <si>
-    <t>Pa1E1</t>
+    <t>Pu1E1</t>
   </si>
   <si>
     <t>Pa1</t>
@@ -1402,7 +1402,7 @@
     <t>Wang_2016_EPHPP</t>
   </si>
   <si>
-    <t>Pa2E1</t>
+    <t>Pu2E1</t>
   </si>
   <si>
     <t>Pa2</t>
@@ -1432,7 +1432,19 @@
     <t>https://doi.org/10.17605/OSF.IO/XA4H8</t>
   </si>
   <si>
-    <t>Pa2E2</t>
+    <t>Pu2E2</t>
+  </si>
+  <si>
+    <t>Pu3E1</t>
+  </si>
+  <si>
+    <t>Pa3</t>
+  </si>
+  <si>
+    <t>Smith_2024_Cortex</t>
+  </si>
+  <si>
+    <t>https://osf.io/br98c/</t>
   </si>
 </sst>
 </file>
@@ -2109,7 +2121,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2153,9 +2165,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2503,11 +2512,11 @@
   <dimension ref="A1:KI69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="74" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="AB31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="AI2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AI51" sqref="AI51"/>
+      <selection pane="bottomRight" activeCell="AI5" sqref="AI5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -2650,7 +2659,7 @@
       <c r="AH1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="19" t="s">
+      <c r="AI1" s="18" t="s">
         <v>33</v>
       </c>
       <c r="AJ1" t="s">
@@ -4557,7 +4566,7 @@
       <c r="AI7" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AJ7" s="10" t="s">
+      <c r="AJ7" s="14" t="s">
         <v>85</v>
       </c>
       <c r="AK7" s="2"/>
@@ -4919,7 +4928,7 @@
       <c r="AI8" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AJ8" s="16" t="s">
+      <c r="AJ8" s="15" t="s">
         <v>98</v>
       </c>
       <c r="AK8" s="2"/>
@@ -5243,7 +5252,7 @@
       <c r="V9" s="2">
         <v>7</v>
       </c>
-      <c r="W9" s="16" t="s">
+      <c r="W9" s="15" t="s">
         <v>106</v>
       </c>
       <c r="X9" s="2"/>
@@ -5278,7 +5287,7 @@
       <c r="AI9" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AJ9" s="16" t="s">
+      <c r="AJ9" s="15" t="s">
         <v>110</v>
       </c>
       <c r="AK9" s="2" t="s">
@@ -6002,10 +6011,10 @@
       <c r="AI11" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="AJ11" s="16" t="s">
+      <c r="AJ11" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="AK11" s="10" t="s">
+      <c r="AK11" s="14" t="s">
         <v>131</v>
       </c>
       <c r="AL11" s="2"/>
@@ -6364,7 +6373,7 @@
       <c r="AI12" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="AJ12" s="16" t="s">
+      <c r="AJ12" s="15" t="s">
         <v>130</v>
       </c>
       <c r="AK12" s="10" t="s">
@@ -6730,7 +6739,7 @@
       <c r="AI13" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="AJ13" s="16" t="s">
+      <c r="AJ13" s="15" t="s">
         <v>149</v>
       </c>
       <c r="AK13" s="2" t="s">
@@ -7098,7 +7107,7 @@
       <c r="AI14" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="AJ14" s="20" t="s">
+      <c r="AJ14" s="19" t="s">
         <v>162</v>
       </c>
       <c r="AK14" s="2" t="s">
@@ -7461,7 +7470,7 @@
       <c r="AI15" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="AJ15" s="21" t="s">
+      <c r="AJ15" s="20" t="s">
         <v>162</v>
       </c>
       <c r="AK15" s="2" t="s">
@@ -12103,7 +12112,7 @@
       <c r="V28" s="2">
         <v>3</v>
       </c>
-      <c r="W28" s="17" t="s">
+      <c r="W28" s="16" t="s">
         <v>229</v>
       </c>
       <c r="X28" s="2"/>
@@ -12139,7 +12148,7 @@
       <c r="AI28" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="AJ28" s="16" t="s">
+      <c r="AJ28" s="15" t="s">
         <v>232</v>
       </c>
       <c r="AK28" s="2"/>
@@ -12846,10 +12855,10 @@
       <c r="AC30" s="2">
         <v>23</v>
       </c>
-      <c r="AD30" s="18" t="s">
+      <c r="AD30" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="AE30" s="18"/>
+      <c r="AE30" s="17"/>
       <c r="AF30" s="2">
         <v>1</v>
       </c>
@@ -12863,7 +12872,7 @@
       <c r="AI30" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="AJ30" s="10" t="s">
+      <c r="AJ30" s="14" t="s">
         <v>252</v>
       </c>
       <c r="AK30" s="2" t="s">
@@ -15634,7 +15643,7 @@
       <c r="AI38" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="AJ38" s="20" t="s">
+      <c r="AJ38" s="19" t="s">
         <v>289</v>
       </c>
       <c r="AK38" s="2" t="s">
@@ -16367,7 +16376,7 @@
       <c r="AJ40" s="14" t="s">
         <v>307</v>
       </c>
-      <c r="AK40" s="16" t="s">
+      <c r="AK40" s="15" t="s">
         <v>308</v>
       </c>
       <c r="AL40" s="2"/>
@@ -17793,10 +17802,10 @@
       <c r="AC44" s="2">
         <v>328</v>
       </c>
-      <c r="AD44" s="18" t="s">
+      <c r="AD44" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="AE44" s="18"/>
+      <c r="AE44" s="17"/>
       <c r="AF44" s="2">
         <v>40</v>
       </c>
@@ -19227,10 +19236,10 @@
       <c r="AC48" s="2">
         <v>380</v>
       </c>
-      <c r="AD48" s="18" t="s">
+      <c r="AD48" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="AE48" s="18"/>
+      <c r="AE48" s="17"/>
       <c r="AF48" s="2">
         <v>32</v>
       </c>
@@ -19242,7 +19251,7 @@
       <c r="AI48" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="AJ48" s="10" t="s">
+      <c r="AJ48" s="14" t="s">
         <v>353</v>
       </c>
       <c r="AK48" s="2" t="s">
@@ -19597,7 +19606,7 @@
       <c r="AI49" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="AJ49" s="16" t="s">
+      <c r="AJ49" s="15" t="s">
         <v>361</v>
       </c>
       <c r="AK49" s="2" t="s">
@@ -21266,13 +21275,13 @@
       <c r="H54" s="7">
         <v>0</v>
       </c>
-      <c r="I54" s="15" t="s">
+      <c r="I54" s="13" t="s">
         <v>396</v>
       </c>
       <c r="J54" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="K54" s="15" t="s">
+      <c r="K54" s="13" t="s">
         <v>398</v>
       </c>
       <c r="L54" s="2">
@@ -21617,13 +21626,13 @@
       <c r="H55" s="7">
         <v>0</v>
       </c>
-      <c r="I55" s="15" t="s">
+      <c r="I55" s="13" t="s">
         <v>396</v>
       </c>
       <c r="J55" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="K55" s="15" t="s">
+      <c r="K55" s="13" t="s">
         <v>398</v>
       </c>
       <c r="L55" s="2">
@@ -21947,13 +21956,27 @@
     </row>
     <row r="56" ht="15.5" spans="1:295">
       <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
+      <c r="B56" s="2">
+        <v>55</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F56" s="4">
+        <v>1</v>
+      </c>
+      <c r="G56" s="7">
+        <v>0</v>
+      </c>
+      <c r="H56" s="4">
+        <v>1</v>
+      </c>
       <c r="I56" s="2"/>
       <c r="J56" s="10"/>
       <c r="K56" s="2"/>
@@ -21980,9 +22003,15 @@
       <c r="AF56" s="2"/>
       <c r="AG56" s="2"/>
       <c r="AH56" s="2"/>
-      <c r="AI56" s="2"/>
-      <c r="AJ56" s="10"/>
-      <c r="AK56" s="2"/>
+      <c r="AI56" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="AJ56" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="AK56" s="2" t="s">
+        <v>175</v>
+      </c>
       <c r="AL56" s="2"/>
       <c r="AM56" s="2"/>
       <c r="AN56" s="2"/>
@@ -22244,10 +22273,14 @@
     </row>
     <row r="57" ht="15.5" spans="1:295">
       <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
+      <c r="B57" s="2">
+        <v>56</v>
+      </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
+      <c r="E57" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -25531,7 +25564,7 @@
       <c r="M69" s="2"/>
     </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:AK55" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:AK57" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <mergeCells count="3">
@@ -25594,6 +25627,7 @@
     <hyperlink ref="AJ52" r:id="rId34" display="https://doi.org/10.3758/s13415-024-01157-0."/>
     <hyperlink ref="AJ54" r:id="rId35" display="https://doi.org/10.17605/OSF.IO/XA4H8" tooltip="https://doi.org/10.17605/OSF.IO/XA4H8"/>
     <hyperlink ref="AJ55" r:id="rId35" display="https://doi.org/10.17605/OSF.IO/XA4H8" tooltip="https://doi.org/10.17605/OSF.IO/XA4H8"/>
+    <hyperlink ref="AJ56" r:id="rId36" display="https://osf.io/br98c/" tooltip="https://osf.io/br98c/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>